<commit_message>
updated final project folder names
</commit_message>
<xml_diff>
--- a/assignments/FinalProject_2023/data_dictionary.xlsx
+++ b/assignments/FinalProject_2023/data_dictionary.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sturrockh/Documents/Work/MEI/DiSARM/GitRepos/spatial-epi-course/course_materials/FinalProject_2021/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erikafoster/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161922DF-8658-DD4B-97F2-CF49AE0E240B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD470CA-AFEA-454E-841B-6CCE0BAEA238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1860" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{21462D38-63D1-654D-8854-FF3410800430}"/>
+    <workbookView xWindow="760" yWindow="560" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{21462D38-63D1-654D-8854-FF3410800430}"/>
   </bookViews>
   <sheets>
     <sheet name="COVID-USA" sheetId="1" r:id="rId1"/>
     <sheet name="Melanoma-USA" sheetId="2" r:id="rId2"/>
-    <sheet name="Malaria-AFG" sheetId="3" r:id="rId3"/>
-    <sheet name="STH-KEN" sheetId="4" r:id="rId4"/>
-    <sheet name="LF-BFA" sheetId="5" r:id="rId5"/>
+    <sheet name="STH-KEN" sheetId="4" r:id="rId3"/>
+    <sheet name="LF-BFA" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
   <si>
     <t>NAME_1</t>
   </si>
@@ -124,48 +123,12 @@
     <t>State population in 2012</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>citation1</t>
-  </si>
-  <si>
     <t>latitude</t>
   </si>
   <si>
     <t>longitude</t>
   </si>
   <si>
-    <t>lower.age</t>
-  </si>
-  <si>
-    <t>upper.age</t>
-  </si>
-  <si>
-    <t>pf.pos</t>
-  </si>
-  <si>
-    <t>examined</t>
-  </si>
-  <si>
-    <t>unique ID for the community</t>
-  </si>
-  <si>
-    <t>citation of source data</t>
-  </si>
-  <si>
-    <t>lowest age of individual included in the sample</t>
-  </si>
-  <si>
-    <t>highest age of individual included in the sample</t>
-  </si>
-  <si>
-    <t>number of individuals testing positive</t>
-  </si>
-  <si>
-    <t>number of individuals tested</t>
-  </si>
-  <si>
     <t>adm1_name</t>
   </si>
   <si>
@@ -181,12 +144,6 @@
     <t>stoolsexaminedgeo</t>
   </si>
   <si>
-    <t>asc_np</t>
-  </si>
-  <si>
-    <t>tri_np</t>
-  </si>
-  <si>
     <t>hk_np</t>
   </si>
   <si>
@@ -205,13 +162,7 @@
     <t>number of stools examined for geohelminths</t>
   </si>
   <si>
-    <t>number of stools testing positive for Ascaris lumbricoides (roundworm)</t>
-  </si>
-  <si>
     <t>number of stools testing positive for hookworm</t>
-  </si>
-  <si>
-    <t>number of stools testing positive for Trichuris trichiura (whipworm)</t>
   </si>
   <si>
     <t>ADM1_NAME</t>
@@ -771,90 +722,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDDFC542-62FB-1B43-A1A1-A7BC39706DD0}">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD7695C2-952E-AB4F-B63E-5EA9E7E8F8DA}">
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD7695C2-952E-AB4F-B63E-5EA9E7E8F8DA}">
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -864,74 +736,58 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -939,11 +795,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDDD649C-0D20-8947-A2A0-EA672B0743AA}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -954,74 +810,74 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>